<commit_message>
Ah yes sending without initializing ESPNOW
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\GIT\ESP32-DRONE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F0DAEE7-0276-4C9A-ADB2-74F38E2DD90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC73F596-E9ED-4655-9AA5-C7271C2C0E9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1617,8 +1617,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70605F78-30C8-4C69-BEBF-95ED07BC628B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AE26" sqref="AE26"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AB13" sqref="AB13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>